<commit_message>
changes in the UI logic to pick up data from risk assesment file
</commit_message>
<xml_diff>
--- a/status_report.xlsx
+++ b/status_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saswatdas/ai_agent_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CAA955-8435-AE40-B276-3359B0BF4A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608F8D3A-FAB3-2841-9371-C5E526A1DF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="1380" windowWidth="26440" windowHeight="14400" xr2:uid="{DDD15A6C-207A-0748-8728-DF4B270F24A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="85">
   <si>
     <t>Project Name</t>
   </si>
@@ -50,15 +50,9 @@
     <t>Planned end date</t>
   </si>
   <si>
-    <t>Planned start date</t>
-  </si>
-  <si>
     <t>Updated</t>
   </si>
   <si>
-    <t>Phase</t>
-  </si>
-  <si>
     <t>Business Value Comment</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t/>
   </si>
   <si>
-    <t>Initiating</t>
-  </si>
-  <si>
     <t>Portfolio manager</t>
   </si>
   <si>
@@ -102,18 +93,12 @@
   </si>
   <si>
     <t>Sandeep Satapathy (GBSSBW)</t>
-  </si>
-  <si>
-    <t>Closing</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Progress &amp;amp; Success:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
 &lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Hypercare successfully completed and ATO signed-off as per plan. Project team dispersed. Closure activities are in progress.&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;The &amp;#39;HVO B7&amp;#39; tool is projected to generate approximately $3 million per annum in tax rebates for Shell, with the value poised to grow as sales of HVO B7 continue to increase.&lt;/li&gt;&lt;/ul&gt;
 &lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Challenges &amp;amp; RTGs:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
 &lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;None&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>Planning</t>
   </si>
   <si>
     <t>&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;&lt;span style="font-size: 10pt;"&gt;Once the data in AMDP production is fixed. AMDP team will inform and work with T&amp;amp;S support to make the appropriate changes in the HVO B7 code to start consuming data from AMDP. Project team already provided hand over to the support team regarding the changes they need to make. &lt;/span&gt;&lt;br /&gt;&lt;br /&gt;&lt;/li&gt;&lt;/ul&gt;</t>
@@ -260,6 +245,158 @@
   <si>
     <t>test1</t>
   </si>
+  <si>
+    <t>Downstream Exchange Product (DSX)</t>
+  </si>
+  <si>
+    <t>PRJ0016435</t>
+  </si>
+  <si>
+    <t>David Gilmour (WYDGIU)</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Progress &amp;amp; Success:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Externalisation:
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Technical &amp;amp; functional readiness on track for Sept; Pilot customer may not be able to participate as internal reorg is taking their focus, still planned to show by end of Aug the demo. Alternative customers identified for pilot if required.&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;ICE Derived data license on the critical path &lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;PEN Test completed without any major or critical findings&lt;/li&gt;&lt;/ul&gt;
+&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Global Support Model: Internal model being discussed with the IT Management. Final step is to go to Owen O&amp;#39;Connell in Sept for approval.&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Henry Hub onboarding onto DSX has begun, planned to complete testing by end of year with a go-live in H1 2026&lt;/li&gt;&lt;/ul&gt;
+&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Challenges &amp;amp; RTG:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Schedule (Red): Externalisation: Market Data Agreements may not be agreed with ICE exchange prior to go-live. Need agreement by end of Aug if we are to stick with the go-live end of Sept.
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;RTG: Legal drafting a letter to reinstate ask, Graham to follow up with a F2F meeting with the exchange.&lt;/li&gt;&lt;/ul&gt;
+&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;n/a&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;Schedule (Red): Externalisation: Market Data Agreements may not be agreed with ICE exchange prior to go-live.  Need agreement by end of Aug if we are to stick with the go-live end of Sept.&lt;/span&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="list-style-type: none; font-size: 10pt;"&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;RTG: Legal drafting a letter to reinstate ask, Graham to follow up with a F2F meeting with the exchange.&lt;/li&gt;&lt;/ul&gt;
+&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;14th Aug -&lt;/strong&gt; DSX v116, AES v5.9 &amp;amp; DSP v2.70 Release is scheduled for Production deployment on Thursday, 14th August. This release includes a set of new features, enhancements, and bug fixes, along with additional changes supporting the Externalization capability, which is targeted to go live later this quarter.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt; &lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;21st Aug -&lt;/strong&gt; A Disaster Recovery (DR) capability proving exercise is scheduled for 21st August as part of our annual operational resilience strategy. This critical activity ensures our ability to recover services during major incidents, supports compliance requirements, and reinforces confidence in our failover and recovery capabilities. For this activity, the focus will be on proving DR capability for DSX, excluding other components (AES &amp;amp; DSP) from this exercise.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;8th July -&lt;/strong&gt; Trading Technologies (TT) released an updated &lt;strong&gt;TTFIX.crt&lt;/strong&gt; file, which contained the public certificates required for connectivity to TT’s FIX endpoint. These certificates are subject to annual renewal and must be updated to maintain uninterrupted service.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;TT recommended that the updated file be implemented &lt;strong&gt;prior to 11th July&lt;/strong&gt;, as the existing certificates were due to expire on that date.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;The update was successfully applied to &lt;strong&gt;AES Production&lt;/strong&gt; on &lt;strong&gt;Tuesday, 8th July at 8 PM UK&lt;/strong&gt;.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt; &lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;17th July -&lt;/strong&gt; Successfully established and enabled AES-to-TT VPN connectivity in Production, transitioning from public internet to a secure VPN channel for enhanced reliability and security.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt; &lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;17th July -&lt;/strong&gt; DSX v115, AES v5.8 &amp;amp; DSP v2.69 were successfully deployed to Production, marking a key milestone in our strategic roadmap. This release delivered new features and enhancements,&lt;strong&gt; &lt;/strong&gt;and also included foundational changes supporting upcoming Externalization and FX Hedging capabilities, both scheduled to go live later this year.&lt;/p&gt;
+&lt;p&gt;&lt;span style="font-size: 11pt; font-family: Aptos, sans-serif;"&gt; &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;Schedule (Red): Externalisation: Market Data Agreements may not be agreed with ICE exchange prior to go-live.  Need agreement by end of Aug if we are to stick with the go-live end of Sept.&lt;/span&gt;&lt;/p&gt;
+&lt;ul&gt;&lt;li style="list-style-type: none; font-size: 10pt;"&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;&lt;span style="font-size: 10pt;"&gt;RTG: Legal drafting a letter to reinstate ask, Graham to follow up with a F2F meeting with the exchange.&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;
+&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;8th July -&lt;/strong&gt; Trading Technologies (TT) released an updated &lt;strong&gt;TTFIX.crt&lt;/strong&gt; file, which contained the public certificates required for connectivity to TT’s FIX endpoint. These certificates are subject to annual renewal and must be updated to maintain uninterrupted service.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;TT recommended that the updated file be implemented &lt;strong&gt;prior to 11th July&lt;/strong&gt;, as the existing certificates were due to expire on that date.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;The update was successfully applied to &lt;strong&gt;AES Production&lt;/strong&gt; on &lt;strong&gt;Tuesday, 8th July at 8 PM UK&lt;/strong&gt;.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt; &lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;17th July -&lt;/strong&gt; Successfully established and enabled AES-to-TT VPN connectivity in Production, transitioning from public internet to a secure VPN channel for enhanced reliability and security.&lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt; &lt;/p&gt;
+&lt;p style="margin: 0in; font-size: 11pt; font-family: Aptos, sans-serif;"&gt;&lt;strong&gt;17th July -&lt;/strong&gt; DSX v115, AES v5.8 &amp;amp; DSP v2.69 were successfully deployed to Production, marking a key milestone in our strategic roadmap. This release delivered new features and enhancements,&lt;strong&gt; &lt;/strong&gt;and also included foundational changes supporting upcoming Externalization and FX Hedging capabilities, both scheduled to go live later this year.&lt;/p&gt;
+&lt;p&gt;&lt;span style="font-size: 11.0pt; font-family: Aptos, sans-serif;"&gt;&lt;br /&gt;&lt;br /&gt;&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Progress &amp;amp; Success:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Externalisation:
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Externalisation name has been agreed with the business (eMarkets) and the external infrastructure for Dev &amp;amp; UAT has been built, Prod in Progress.&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Externalisation - MVP Web App developed, Integration testing completed, business to review and continue business testing as part of the DSX releases. Business are likely to show an external client at the end of the month a demo (Shell location).&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Externalisation: Development completed with the external authentication platform (CIPM), now in UAT.&lt;/li&gt;&lt;/ul&gt;
+&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Global Support Model: Internal model being discussed with the IT Management&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;AES Tech Lead position is now filled&lt;/li&gt;&lt;/ul&gt;
+&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Challenges &amp;amp; RTG:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Schedule (Amber): Externalisation: Security developments slightly behind plan, impacting the PEN test timeline, risk that if there are findings in the PEN test we may not go live in Sept. RTG track progress and see if additional resources would help improve the delivery.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;UAT testing and PROD deployment of DSX v115, AES v5.8, DSP v70&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;successful PROD Deployment of -  DSX v114, AES v5.7, DSP v69&lt;/p&gt;
+&lt;p&gt; &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Progress &amp;amp; Success:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Externalisation name has been agreed with the business (eMarkets) and the external infrastructure for Dev &amp;amp; UAT has been built, Prod in Progress.&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Externalisation - MVP Web App developed, Testing will start in July with the business and be demonstrated to the pilot customer end of July.&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Global Support Model: ABC proposal received and being assessed along with an updated internal model&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;IRM Control work now completed and now supported by SOM rather than the project. Now can be operated by SOM and project under agreement to co - operate &lt;/li&gt;&lt;/ul&gt;
+&lt;p&gt;&lt;span style="font-size: 10pt;"&gt;&lt;strong&gt;Challenges &amp;amp; RTG:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li style="font-size: 10pt;"&gt;Schedule (Amber): FX hedging [Green]: FX Hedging Go live now replanned after receiving revised dates from Bloomberg&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Resources (Amber): Hiring of AES tech lead remains challenging RTG Plan: Continue to Onboard Niche recruiters&lt;/li&gt;&lt;li style="font-size: 10pt;"&gt;Schedule (Amber): Externalisation: Security developments slightly behind plan, impacting the PEN test timeline, risk that if there are findings in the PEN test we may not go live in Sept. RTG track progress and see if additional resources would help improve the delivery.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;FX hedging [Red]: Bloomberg have communicated a Q3 delivery timeline.&lt;/div&gt;
+&lt;div&gt;RTG Plan: escalated to D. Gardner (FXGO PO) but no change in plan.&lt;/div&gt;
+&lt;div&gt;Externalisation: Security developments slightly behind plan, impacting the PEN test timeline, risk that if there are findings in the PEN test we may not go live in Sept.  RTG  track progress and see if additional resources would help improve the delivery.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;UAT testing and PROD deployment of DSX v114, AES v5.7, DSP v69&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;successful PROD Deployment of -  DSX v113,  AES v5.6, AES DSP v68&lt;/p&gt;
+&lt;p&gt;Externalization Node infrastructure now deployed&lt;/p&gt;
+&lt;p&gt; &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Deal Entry Portal (DEP)</t>
+  </si>
+  <si>
+    <t>PRJ0022729</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Progress &amp;amp; Success:&lt;/strong&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li&gt;New Houston based developer has joined the team, this is the start of the team build-out in the US to support the eMarketplace replacement work&lt;/li&gt;&lt;li&gt;European Spread Options successfully deployed to production&lt;/li&gt;&lt;li&gt;Phase 1 structuring work deployed with additional manual deal entry products supported&lt;/li&gt;&lt;li&gt;Henry Hub project kick-off completed&lt;/li&gt;&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Challenges &amp;amp; RTC:&lt;/strong&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li&gt;Morgan Stanley (Euronext) connectivity not working and response from the bank have been lacklustre, this has been escalated to the business to put pressure on resolution, we have some conference calls now arranged between the network teams&lt;/li&gt;&lt;li&gt;Additional BA &amp;amp; Dev need to be hired into Houston and resume quality remains unsatisfactory, this will extend times to build the team&lt;/li&gt;&lt;li&gt;Endur resources have not arrived as anticipated as they have been prioritised by the cc onto other projects.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Costs are in line with budgets&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Senior Developer has started in Houston&lt;/p&gt;
+&lt;p&gt;Looking to hire an additional developer and BA in Houston to support the eMarketplace work and wider DSX program adoption in US&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Most deliverables remain on track&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Progress &amp;amp; Success:&lt;/strong&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li&gt;eMarketplace replacement budget approved for 2025 by PDS council&lt;/li&gt;&lt;li&gt;Mobile work rolled out to all traders (subject to permisisoning)&lt;/li&gt;&lt;li&gt;Structuring work has entered UAT testing as DEX work has completed, Planned to complete UAT by 18th July, Go-live date still be discussed with DEX SOM &amp;amp; their release dates&lt;/li&gt;&lt;li&gt;Morgan Stanley (Euronext) development complete, waiting on Firewalls change to finalise the E2E connectivity - requested via ServiceNow.&lt;/li&gt;&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Challenges &amp;amp; RTC:&lt;/strong&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li&gt;None&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We remain in an amber state as we cannot staff the team in Houston.  &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Costs have moved back in line with budget following the release of contingency&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Senior Developer role has been identified and will start on 4th Aug.&lt;/p&gt;
+&lt;p&gt;Looking to hire an additional developer and BA in Houston to support the eMarketplace work and wider DSX program adoption in US&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Scope returns to green following agreement by PDS to increase scope to include eMarketplace&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Progress &amp;amp; Success:&lt;/strong&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li&gt;Compete the ADA and Norske work (subject to services available from ADA)&lt;/li&gt;&lt;li&gt;Review the Fees work with ETD Ops for both the broker charges and TT market data reports&lt;/li&gt;&lt;li&gt;EMarketplace PoC complete, conversations continue on scope (Crude in or out?) and fully functionality required. Get agreement on starting eMarketplace replacement and agree scope.&lt;/li&gt;&lt;/ul&gt;
+&lt;p&gt;&lt;strong&gt;Challenges &amp;amp; RTC:&lt;/strong&gt;&lt;/p&gt;
+&lt;ul style="list-style-position: inside;"&gt;&lt;li&gt;Hiring Python developer into Houston is remaining challenges with few CVs looking suitable, we are being supported by CC&lt;/li&gt;&lt;li&gt;Additional RPLN&amp;#39;s raised for eMarketplace replacement team,going through SVP approval, needs additional funding or contingency releasing&lt;/li&gt;&lt;li&gt;Scope (AMBER): eMarketplace scope to be agreed RTG: Cat to help Richard and Stacy make a decision on scope of eMarketplace..&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;We remain in an amber state as we cannot staff the team in Houston.  Costs are high as we are setting up a US team to support the eMarketplace work.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Cost are high as LE contains additional staff costs to setup Houston dev team for eMarketplace development.  Additional funding/contingency being requested.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hiring into Houston remain to be a challenge we have not yet identified a suitable candidate for the Senior Developer role.  We are working with the CC leads and recruitment to try and get suitable candidates from the market. RTG: Action with Tamia to find appropriate resource.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Scope (AMBER): eMarketplace scope to be agreed RTG: Cat to help Richard and Stacy make a decision on scope of eMarketplace..&lt;/p&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -268,7 +405,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,13 +419,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -314,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -327,6 +477,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CC5780-0885-9F4C-B9E7-A42EDA54B6F5}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:O171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F18" sqref="F18:F171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,12 +829,17 @@
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.1640625" customWidth="1"/>
     <col min="5" max="5" width="18" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" customWidth="1"/>
+    <col min="14" max="14" width="75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -724,436 +885,1220 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E2" s="2">
         <v>46034.708333333336</v>
       </c>
-      <c r="F2" s="2">
-        <v>45674.333333333336</v>
-      </c>
-      <c r="G2" s="2">
-        <v>45901.728564814817</v>
+      <c r="F2" s="6">
+        <v>45905.395578703705</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="372" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="2">
         <v>46034.708333333336</v>
       </c>
-      <c r="F3" s="2">
-        <v>45674.333333333336</v>
-      </c>
-      <c r="G3" s="2">
-        <v>45901.501423611109</v>
+      <c r="F3" s="6">
+        <v>45904.307430555556</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2">
         <v>46034.708333333336</v>
       </c>
-      <c r="F4" s="2">
-        <v>45674.333333333336</v>
-      </c>
-      <c r="G4" s="2">
-        <v>45870.501863425925</v>
+      <c r="F4" s="6">
+        <v>45904.3203587963</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2">
         <v>46034.708333333336</v>
       </c>
-      <c r="F5" s="2">
-        <v>45674.333333333336</v>
-      </c>
-      <c r="G5" s="2">
-        <v>45839.501863425925</v>
+      <c r="F5" s="6">
+        <v>45903.785520833335</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E6" s="2">
         <v>46477.708333333336</v>
       </c>
-      <c r="F6" s="2">
-        <v>45686.333333333336</v>
-      </c>
-      <c r="G6" s="2">
-        <v>45901.257870370369</v>
+      <c r="F6" s="6">
+        <v>45905.101770833331</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" s="2">
         <v>46387.708333333336</v>
       </c>
-      <c r="F7" s="2">
-        <v>45686.333333333336</v>
-      </c>
-      <c r="G7" s="2">
-        <v>45901.502523148149</v>
+      <c r="F7" s="6">
+        <v>45902.841087962966</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2">
         <v>46387.708333333336</v>
       </c>
-      <c r="F8" s="2">
-        <v>45686.333333333336</v>
-      </c>
-      <c r="G8" s="2">
-        <v>45870.501944444448</v>
+      <c r="F8" s="6">
+        <v>45901.404849537037</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2">
         <v>46022.708333333336</v>
       </c>
-      <c r="F9" s="2">
-        <v>45686.333333333336</v>
-      </c>
-      <c r="G9" s="2">
-        <v>45839.501932870371</v>
+      <c r="F9" s="6">
+        <v>45901.326550925929</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="2">
+        <v>46022.708333333336</v>
+      </c>
+      <c r="F10" s="6">
+        <v>45901.210474537038</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2">
+        <v>46022.708333333336</v>
+      </c>
+      <c r="F11" s="6">
+        <v>45901.316435185188</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="2">
+        <v>46022.708333333336</v>
+      </c>
+      <c r="F12" s="6">
+        <v>45904.648796296293</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2">
+        <v>46022.708333333336</v>
+      </c>
+      <c r="F13" s="6">
+        <v>45901.318425925929</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2">
+        <v>46118.708333333336</v>
+      </c>
+      <c r="F14" s="6">
+        <v>45901.724537037036</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="187" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="2">
+        <v>46118.708333333336</v>
+      </c>
+      <c r="F15" s="6">
+        <v>45905.641030092593</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="204" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2">
+        <v>46118.708333333336</v>
+      </c>
+      <c r="F16" s="6">
+        <v>45903.489340277774</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="2">
+        <v>46118.708333333336</v>
+      </c>
+      <c r="F17" s="6">
+        <v>45901.728564814817</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F91" s="6"/>
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F92" s="6"/>
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F94" s="6"/>
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F95" s="6"/>
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F96" s="6"/>
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F97" s="6"/>
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F98" s="6"/>
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F99" s="6"/>
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F100" s="6"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F101" s="6"/>
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F102" s="6"/>
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F103" s="6"/>
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F104" s="6"/>
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F105" s="6"/>
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F106" s="6"/>
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F107" s="6"/>
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F108" s="6"/>
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F109" s="6"/>
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F110" s="6"/>
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F111" s="6"/>
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F112" s="6"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F113" s="6"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F114" s="6"/>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F115" s="6"/>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F116" s="6"/>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F117" s="6"/>
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F118" s="6"/>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F119" s="6"/>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F120" s="6"/>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F121" s="6"/>
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F122" s="6"/>
+    </row>
+    <row r="123" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F123" s="6"/>
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F124" s="6"/>
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F125" s="6"/>
+    </row>
+    <row r="126" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F126" s="6"/>
+    </row>
+    <row r="127" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F127" s="6"/>
+    </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F128" s="7"/>
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F129" s="6"/>
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F130" s="6"/>
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F131" s="6"/>
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F132" s="6"/>
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F133" s="6"/>
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F134" s="6"/>
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F135" s="6"/>
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F136" s="6"/>
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F137" s="6"/>
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F138" s="6"/>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F139" s="6"/>
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F140" s="6"/>
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F141" s="6"/>
+    </row>
+    <row r="142" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F142" s="6"/>
+    </row>
+    <row r="143" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F143" s="6"/>
+    </row>
+    <row r="144" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F144" s="6"/>
+    </row>
+    <row r="145" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F145" s="6"/>
+    </row>
+    <row r="146" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F146" s="6"/>
+    </row>
+    <row r="147" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F147" s="6"/>
+    </row>
+    <row r="148" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F148" s="6"/>
+    </row>
+    <row r="149" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F149" s="6"/>
+    </row>
+    <row r="150" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F150" s="6"/>
+    </row>
+    <row r="151" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F151" s="6"/>
+    </row>
+    <row r="152" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F152" s="6"/>
+    </row>
+    <row r="153" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F153" s="6"/>
+    </row>
+    <row r="154" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F154" s="6"/>
+    </row>
+    <row r="155" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F155" s="6"/>
+    </row>
+    <row r="156" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F156" s="6"/>
+    </row>
+    <row r="157" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F157" s="6"/>
+    </row>
+    <row r="158" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F158" s="6"/>
+    </row>
+    <row r="159" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F159" s="6"/>
+    </row>
+    <row r="160" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F160" s="6"/>
+    </row>
+    <row r="161" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F161" s="6"/>
+    </row>
+    <row r="162" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F162" s="6"/>
+    </row>
+    <row r="163" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F163" s="6"/>
+    </row>
+    <row r="164" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F164" s="6"/>
+    </row>
+    <row r="165" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F165" s="6"/>
+    </row>
+    <row r="166" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F166" s="6"/>
+    </row>
+    <row r="167" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F167" s="6"/>
+    </row>
+    <row r="168" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F168" s="6"/>
+    </row>
+    <row r="169" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F169" s="6"/>
+    </row>
+    <row r="170" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F170" s="6"/>
+    </row>
+    <row r="171" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F171" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>